<commit_message>
Ensure the Daily Driver Report uses only verified employee data sources
Refactor reports_processor.py to validate driver data against ELIST/JLIST, add logging, and update trend reports.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b83b866c-5b8f-4d82-9fde-612e7a355315
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f2699832-8135-4557-9ec0-8d4d723b9ba2/6cae282f-4da6-4652-b741-314e4141184c.jpg
</commit_message>
<xml_diff>
--- a/exports/daily_reports/2025-05-16_DailyDriverReport.xlsx
+++ b/exports/daily_reports/2025-05-16_DailyDriverReport.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,1595 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>employee_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>phone</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>division</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>job_title</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>asset</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>arrival</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>departure</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Carlos Flores</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>240163</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>(817) 655-0366</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>F-03</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>08:02 AM</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Miguel Perez Ramirez</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>240421</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>(682) 386-9790</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>F-65</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Early Departure</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>07:15 AM</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>15:10 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Daniel Farias</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>440317</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>RAM-68</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>06:52 AM</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Salvador Hernandez-Espinoza</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>240264</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>(817) 566-5847</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>HD-15</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>06:55 AM</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Joshua Smith</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>440114</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>jsmith@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>(832) 576-0854</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>HD-76</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>08:03 AM</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Juan Reyes Ibarra</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>440365</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>(832) 677-5615</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>HD-07</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>06:56 AM</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Faustino Mendoza</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>240770</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>emanuelmartinez0707@gmail.com</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>(469) 818-3418</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>ET-19</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>06:58 AM</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Norberto Lopez</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>240642</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>(214) 315-6046</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>RAM-09</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>06:51 AM</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Jonathan Salinas</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>440187</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>jonathansalinas1029@gmail.com</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>(979) 525-9184</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>F-11</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>06:59 AM</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Stephanie Santos-Gonzalez</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>440243</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>(346) 357-4014</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>TRK-22</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>06:46 AM</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Karla Reyes</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>200008</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>kreyes@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>(682) 701-4439</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>F-35</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>06:58 AM</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Argelio Padilla</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>440113</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>(832) 461-7833</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>ET-61</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>07:03 AM</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Jose Garcia</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>240733</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>joseluisg254@icloud.com</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>(469) 439-7316</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>HD-28</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>06:56 AM</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Jesus Alvarez</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>240472</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>jesusalvarez1724@gmail.co</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>(682) 715-5097</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>HD-54</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>07:02 AM</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Roy Ramirez-Rodriguez</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>440075</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>(956) 400-0837</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>RAM-63</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>06:56 AM</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Audrey Saldana</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>210063</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>asaldana@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>(972) 816-9867</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>TRK-24</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>06:55 AM</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Juan Beltran</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>440392</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>(346) 283-3609</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>ET-72</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>06:45 AM</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Arturo Ramirez Vazquez</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>440376</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>(346) 772-7938</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>RAM-92</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>06:58 AM</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Armando Valdez-Reivera</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>240312</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>(817) 300-8296</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>RAM-20</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>06:58 AM</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Jose Salazar Moreno</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>240706</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>mauriciosalazar1019@gmail.com</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>(418) 117-3166</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>F-77</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>07:01 AM</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Alejandro Castaneda</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>240803</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>alejandrocastaneda04@icloud.com</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>(817) 262-1850</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>ET-81</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>06:53 AM</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Howard Wright</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>240591</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>(214) 325-3072</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>RAM-37</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>07:01 AM</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Pablo Flores</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>440412</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>(936) 257-2704</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>HD-56</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>06:58 AM</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Domingo Hernandez-Santos</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>240425</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>domingoh865@gmail.com</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>RAM-21</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>07:15 AM</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Vaibhav Dhamangaonkar</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>410007</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>vdhamangaonkar@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>(469) 740-1645</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>F-72</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Early Departure</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>06:54 AM</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>15:46 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Gregorio Sanchez-Leal</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>440184</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>(346) 255-1094</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>F-96</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>07:59 AM</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Ramiro Vazquez De La Cruz</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>240624</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>rvazquez@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>(469) 684-0787</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>F-81</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>06:45 AM</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Terry Franklin</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>210017</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>tfranklin@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>(903) 754-9572</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>ET-25</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>08:07 AM</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Juan Gonzalez</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>440058</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>(713) 791-3143</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>TRK-71</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>06:46 AM</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Jose Hernandez</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>440275</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>(346) 243-2013</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>ET-06</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>08:02 AM</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Seyedalireza Taghavi</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>800074</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>staghavi@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>(210) 741-2348</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>F-21</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>07:35 AM</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Alejandro Abarca Paramo</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>310000</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>aabarca@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>(210) 396-9739</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>TRK-36</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>06:57 AM</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Lisandro Alvarado Alvarado</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>240766</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>maxilisandro12345@gmail.com</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>(469) 956-0159</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>RAM-51</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>06:47 AM</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Christopher Belflower</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>800033</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>cbelflower@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>(651) 402-1777</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>RAM-61</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>07:03 AM</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Zabih Kocer</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>210005</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>zkocer@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>(202) 999-0555</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>TRK-52</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>06:55 AM</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Ramon Reyes</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>240070</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>rr193652@gmail.com</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>(410) 493-7614</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>HD-55</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>07:05 AM</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Cruz Talamantes</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>440349</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>(832) 759-1419</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>HD-83</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>06:47 AM</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Miguel Flores Amezquita</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>240620</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>(214) 447-5459</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>TRK-29</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>06:47 AM</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Jaime Salas Balleza</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>340040</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>(432) 260-9052</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>F-49</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>06:59 AM</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Graciela Villa Fraga</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>800046</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>vvilla@ragleinc.com</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>(817) 680-0754</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>ET-85</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>06:53 AM</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enhance daily reports with data validation, analytics and complete output
Adds new activity tracking, generates integrity checks, improves reports and fixes bugs.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b83b866c-5b8f-4d82-9fde-612e7a355315
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f2699832-8135-4557-9ec0-8d4d723b9ba2/3e85b7b8-1ef7-40e0-99b0-288df767b503.jpg
</commit_message>
<xml_diff>
--- a/exports/daily_reports/2025-05-16_DailyDriverReport.xlsx
+++ b/exports/daily_reports/2025-05-16_DailyDriverReport.xlsx
@@ -483,12 +483,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Christopher Thomas</t>
+          <t>Mark Thompson</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TRK-1011</t>
+          <t>TRK-1015</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -498,22 +498,22 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>06:30 AM</t>
+          <t>06:00 AM</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>03:30 PM</t>
+          <t>03:00 PM</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>06:29 AM</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>03:33 PM</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -526,37 +526,37 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Matthew Harris</t>
+          <t>Christopher Thomas</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TRK-1013</t>
+          <t>TRK-1011</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>North Dallas Site</t>
+          <t>Downtown Construction</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>06:45 AM</t>
+          <t>06:30 AM</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>03:45 PM</t>
+          <t>03:30 PM</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>06:52 AM</t>
+          <t>06:29 AM</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>03:37 PM</t>
+          <t>03:33 PM</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -569,37 +569,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mark Thompson</t>
+          <t>John Smith</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>TRK-1015</t>
+          <t>TRK-1001</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Downtown Construction</t>
+          <t>North Dallas Site</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>06:00 AM</t>
+          <t>06:30 AM</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>03:00 PM</t>
+          <t>03:30 PM</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>06:25 AM</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>03:35 PM</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -612,107 +612,107 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>William Brown</t>
+          <t>Richard Wilson</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>TRK-1004</t>
+          <t>TRK-1007</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Richardson Development</t>
+          <t>Downtown Construction</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>06:30 AM</t>
+          <t>06:15 AM</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>03:30 PM</t>
+          <t>03:15 PM</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>06:32 AM</t>
+          <t>06:14 AM</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>02:54 PM</t>
+          <t>03:18 PM</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Early End</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>36 minutes early</t>
-        </is>
-      </c>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Richard Wilson</t>
+          <t>William Brown</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TRK-1007</t>
+          <t>TRK-1004</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Downtown Construction</t>
+          <t>Richardson Development</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>06:15 AM</t>
+          <t>06:30 AM</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>03:15 PM</t>
+          <t>03:30 PM</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>06:14 AM</t>
+          <t>06:32 AM</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>03:18 PM</t>
+          <t>02:54 PM</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>On Time</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr"/>
+          <t>Early End</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>36 minutes early</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Anthony Martin</t>
+          <t>Thomas Taylor</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>TRK-1014</t>
+          <t>TRK-1009</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>West Plano Project</t>
+          <t>North Dallas Site</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -727,24 +727,20 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>07:16 AM</t>
+          <t>06:43 AM</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>03:58 PM</t>
+          <t>03:52 PM</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Late</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>16 minutes late</t>
-        </is>
-      </c>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -796,149 +792,145 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Charles Anderson</t>
+          <t>Joseph Moore</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>TRK-1010</t>
+          <t>TRK-1008</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>West Plano Project</t>
+          <t>Richardson Development</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>06:00 AM</t>
+          <t>06:30 AM</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>03:00 PM</t>
+          <t>03:30 PM</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>06:05 AM</t>
+          <t>06:55 AM</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>02:48 PM</t>
+          <t>03:25 PM</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>On Time</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr"/>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>25 minutes late</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Michael Johnson</t>
+          <t>Matthew Harris</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>TRK-1002</t>
+          <t>TRK-1013</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>West Plano Project</t>
+          <t>North Dallas Site</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>06:00 AM</t>
+          <t>06:45 AM</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>03:00 PM</t>
+          <t>03:45 PM</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>06:18 AM</t>
+          <t>06:52 AM</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>03:07 PM</t>
+          <t>03:37 PM</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Late</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>18 minutes late</t>
-        </is>
-      </c>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Robert Williams</t>
+          <t>David Miller</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>TRK-1003</t>
+          <t>TRK-1006</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Downtown Construction</t>
+          <t>West Plano Project</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>07:00 AM</t>
+          <t>06:45 AM</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>04:00 PM</t>
+          <t>03:45 PM</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>07:28 AM</t>
+          <t>06:47 AM</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>03:45 PM</t>
+          <t>03:42 PM</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Late</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>28 minutes late</t>
-        </is>
-      </c>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>David Miller</t>
+          <t>Michael Johnson</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>TRK-1006</t>
+          <t>TRK-1002</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -948,40 +940,44 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>06:45 AM</t>
+          <t>06:00 AM</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>03:45 PM</t>
+          <t>03:00 PM</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>06:47 AM</t>
+          <t>06:18 AM</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>03:42 PM</t>
+          <t>03:07 PM</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>On Time</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr"/>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>18 minutes late</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Joseph Moore</t>
+          <t>Daniel Jackson</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TRK-1008</t>
+          <t>TRK-1012</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -991,49 +987,45 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>06:30 AM</t>
+          <t>06:15 AM</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>03:30 PM</t>
+          <t>03:15 PM</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>06:55 AM</t>
+          <t>06:16 AM</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>03:25 PM</t>
+          <t>03:12 PM</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Late</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>25 minutes late</t>
-        </is>
-      </c>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Thomas Taylor</t>
+          <t>Robert Williams</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>TRK-1009</t>
+          <t>TRK-1003</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>North Dallas Site</t>
+          <t>Downtown Construction</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1048,98 +1040,106 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>06:43 AM</t>
+          <t>07:28 AM</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>03:52 PM</t>
+          <t>03:45 PM</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>On Time</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr"/>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>28 minutes late</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Daniel Jackson</t>
+          <t>Anthony Martin</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>TRK-1012</t>
+          <t>TRK-1014</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Richardson Development</t>
+          <t>West Plano Project</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>06:15 AM</t>
+          <t>07:00 AM</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>03:15 PM</t>
+          <t>04:00 PM</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>06:16 AM</t>
+          <t>07:16 AM</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>03:12 PM</t>
+          <t>03:58 PM</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>On Time</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr"/>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>16 minutes late</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>John Smith</t>
+          <t>Charles Anderson</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>TRK-1001</t>
+          <t>TRK-1010</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>North Dallas Site</t>
+          <t>West Plano Project</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>06:30 AM</t>
+          <t>06:00 AM</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>03:30 PM</t>
+          <t>03:00 PM</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>06:25 AM</t>
+          <t>06:05 AM</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>03:35 PM</t>
+          <t>02:48 PM</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">

</xml_diff>

<commit_message>
Ensure daily reports use only verified driver data for enhanced integrity
Implements driver data validation, report rebuild, and audit logging for daily reports in exports/ and reports/ directories.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b83b866c-5b8f-4d82-9fde-612e7a355315
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f2699832-8135-4557-9ec0-8d4d723b9ba2/3e85b7b8-1ef7-40e0-99b0-288df767b503.jpg
</commit_message>
<xml_diff>
--- a/exports/daily_reports/2025-05-16_DailyDriverReport.xlsx
+++ b/exports/daily_reports/2025-05-16_DailyDriverReport.xlsx
@@ -483,17 +483,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mark Thompson</t>
+          <t>Charles Anderson</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TRK-1015</t>
+          <t>TRK-1010</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Downtown Construction</t>
+          <t>West Plano Project</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -508,12 +508,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>06:05 AM</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>02:48 PM</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -526,12 +526,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Christopher Thomas</t>
+          <t>Mark Thompson</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TRK-1011</t>
+          <t>TRK-1015</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -541,22 +541,22 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>06:30 AM</t>
+          <t>06:00 AM</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>03:30 PM</t>
+          <t>03:00 PM</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>06:29 AM</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>03:33 PM</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -569,12 +569,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>John Smith</t>
+          <t>James Davis</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>TRK-1001</t>
+          <t>TRK-1005</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -584,83 +584,91 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>06:30 AM</t>
+          <t>06:00 AM</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>03:30 PM</t>
+          <t>03:00 PM</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>06:25 AM</t>
+          <t>07:03 AM</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>03:35 PM</t>
+          <t>03:12 PM</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>On Time</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr"/>
+          <t>Not On Job</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>At incorrect location: North Richland Hills</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Richard Wilson</t>
+          <t>Anthony Martin</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>TRK-1007</t>
+          <t>TRK-1014</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Downtown Construction</t>
+          <t>West Plano Project</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>06:15 AM</t>
+          <t>07:00 AM</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>03:15 PM</t>
+          <t>04:00 PM</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>06:14 AM</t>
+          <t>07:16 AM</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>03:18 PM</t>
+          <t>03:58 PM</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>On Time</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr"/>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>16 minutes late</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>William Brown</t>
+          <t>Daniel Jackson</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TRK-1004</t>
+          <t>TRK-1012</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -670,69 +678,65 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>06:30 AM</t>
+          <t>06:15 AM</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>03:30 PM</t>
+          <t>03:15 PM</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>06:32 AM</t>
+          <t>06:16 AM</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>02:54 PM</t>
+          <t>03:12 PM</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Early End</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>36 minutes early</t>
-        </is>
-      </c>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Thomas Taylor</t>
+          <t>Christopher Thomas</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>TRK-1009</t>
+          <t>TRK-1011</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>North Dallas Site</t>
+          <t>Downtown Construction</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>07:00 AM</t>
+          <t>06:30 AM</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>04:00 PM</t>
+          <t>03:30 PM</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>06:43 AM</t>
+          <t>06:29 AM</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>03:52 PM</t>
+          <t>03:33 PM</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -745,174 +749,174 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>James Davis</t>
+          <t>William Brown</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>TRK-1005</t>
+          <t>TRK-1004</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>North Dallas Site</t>
+          <t>Richardson Development</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>06:00 AM</t>
+          <t>06:30 AM</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>03:00 PM</t>
+          <t>03:30 PM</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>07:03 AM</t>
+          <t>06:32 AM</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>03:12 PM</t>
+          <t>02:54 PM</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Not On Job</t>
+          <t>Early End</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>At incorrect location: North Richland Hills</t>
+          <t>36 minutes early</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Joseph Moore</t>
+          <t>Richard Wilson</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>TRK-1008</t>
+          <t>TRK-1007</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Richardson Development</t>
+          <t>Downtown Construction</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>06:30 AM</t>
+          <t>06:15 AM</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>03:30 PM</t>
+          <t>03:15 PM</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>06:55 AM</t>
+          <t>06:14 AM</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>03:25 PM</t>
+          <t>03:18 PM</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Late</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>25 minutes late</t>
-        </is>
-      </c>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Matthew Harris</t>
+          <t>Joseph Moore</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>TRK-1013</t>
+          <t>TRK-1008</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>North Dallas Site</t>
+          <t>Richardson Development</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>06:45 AM</t>
+          <t>06:30 AM</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>03:45 PM</t>
+          <t>03:30 PM</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>06:52 AM</t>
+          <t>06:55 AM</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>03:37 PM</t>
+          <t>03:25 PM</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>On Time</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr"/>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>25 minutes late</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>David Miller</t>
+          <t>Thomas Taylor</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>TRK-1006</t>
+          <t>TRK-1009</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>West Plano Project</t>
+          <t>North Dallas Site</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>06:45 AM</t>
+          <t>07:00 AM</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>03:45 PM</t>
+          <t>04:00 PM</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>06:47 AM</t>
+          <t>06:43 AM</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>03:42 PM</t>
+          <t>03:52 PM</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -925,84 +929,80 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Michael Johnson</t>
+          <t>John Smith</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>TRK-1002</t>
+          <t>TRK-1001</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>West Plano Project</t>
+          <t>North Dallas Site</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>06:00 AM</t>
+          <t>06:30 AM</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>03:00 PM</t>
+          <t>03:30 PM</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>06:18 AM</t>
+          <t>06:25 AM</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>03:07 PM</t>
+          <t>03:35 PM</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Late</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>18 minutes late</t>
-        </is>
-      </c>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Daniel Jackson</t>
+          <t>David Miller</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TRK-1012</t>
+          <t>TRK-1006</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Richardson Development</t>
+          <t>West Plano Project</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>06:15 AM</t>
+          <t>06:45 AM</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>03:15 PM</t>
+          <t>03:45 PM</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>06:16 AM</t>
+          <t>06:47 AM</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>03:12 PM</t>
+          <t>03:42 PM</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1015,59 +1015,55 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Robert Williams</t>
+          <t>Matthew Harris</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>TRK-1003</t>
+          <t>TRK-1013</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Downtown Construction</t>
+          <t>North Dallas Site</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>07:00 AM</t>
+          <t>06:45 AM</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>04:00 PM</t>
+          <t>03:45 PM</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>07:28 AM</t>
+          <t>06:52 AM</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>03:45 PM</t>
+          <t>03:37 PM</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Late</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>28 minutes late</t>
-        </is>
-      </c>
+          <t>On Time</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Anthony Martin</t>
+          <t>Michael Johnson</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>TRK-1014</t>
+          <t>TRK-1002</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1077,22 +1073,22 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>07:00 AM</t>
+          <t>06:00 AM</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>04:00 PM</t>
+          <t>03:00 PM</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>07:16 AM</t>
+          <t>06:18 AM</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>03:58 PM</t>
+          <t>03:07 PM</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1102,52 +1098,56 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>16 minutes late</t>
+          <t>18 minutes late</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Charles Anderson</t>
+          <t>Robert Williams</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>TRK-1010</t>
+          <t>TRK-1003</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>West Plano Project</t>
+          <t>Downtown Construction</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>06:00 AM</t>
+          <t>07:00 AM</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>03:00 PM</t>
+          <t>04:00 PM</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>06:05 AM</t>
+          <t>07:28 AM</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>02:48 PM</t>
+          <t>03:45 PM</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>On Time</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr"/>
+          <t>Late</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>28 minutes late</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>